<commit_message>
Update Manual Security Checks.xlsx
</commit_message>
<xml_diff>
--- a/Manual Security Checks.xlsx
+++ b/Manual Security Checks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myresources.deloitte.com/personal/eberruttomorales_deloitte_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxi\Documents\GitHub\HunterXL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="309" documentId="13_ncr:1_{CA6ECF4B-E6C8-485C-A3D1-4C7D5894A261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16562CCD-EAC7-451B-BF9C-0630EC2583B4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E045E5-90F6-4194-A5DE-5BEB4C209A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Testing WebApp" sheetId="10" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="111">
   <si>
     <t>Enumeration in login</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>Malware (Eicar) can be uploaded</t>
-  </si>
-  <si>
-    <t>IDORs</t>
   </si>
   <si>
     <r>
@@ -159,9 +156,6 @@
     <t>Autentication/Session (Grey Box)</t>
   </si>
   <si>
-    <t>Business Logic</t>
-  </si>
-  <si>
     <t>Password Policy (Grey Box)</t>
   </si>
   <si>
@@ -308,9 +302,6 @@
   </si>
   <si>
     <t>Server header version or similar</t>
-  </si>
-  <si>
-    <t>Autorize Plugin on Burp Pro</t>
   </si>
   <si>
     <t>Cookie/Tokens values disclosure sensite information</t>
@@ -622,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -704,9 +695,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -794,7 +782,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1090,687 +1078,665 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C90125-D710-4EF2-B356-32A46CE0C44A}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" style="37" customWidth="1"/>
-    <col min="3" max="3" width="47.6640625" style="37" customWidth="1"/>
+    <col min="2" max="2" width="69.44140625" style="36" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" style="36" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="38" t="s">
+      <c r="A1" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>77</v>
+      <c r="C1" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="49"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
+        <v>34</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
+        <v>73</v>
+      </c>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
+        <v>104</v>
+      </c>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="36"/>
+      <c r="B14" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="35"/>
       <c r="D14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="36"/>
+      <c r="A15" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="35"/>
       <c r="D15" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="36"/>
+      <c r="B17" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="35"/>
       <c r="D17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="36"/>
+      <c r="B18" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="35"/>
       <c r="D18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="36"/>
+      <c r="B19" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="35"/>
       <c r="D19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="36"/>
+      <c r="B20" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="35"/>
       <c r="D20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
+        <v>110</v>
+      </c>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
       <c r="D23" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" s="36"/>
+        <v>109</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="35"/>
       <c r="D24" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
+        <v>38</v>
+      </c>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="36"/>
+      <c r="B26" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="35"/>
       <c r="D26" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C27" s="36"/>
+      <c r="B27" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="35"/>
       <c r="D27" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" s="36"/>
+      <c r="B28" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="35"/>
       <c r="D28" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="36"/>
+      <c r="B29" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="35"/>
       <c r="D29" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" s="36"/>
+      <c r="B30" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="35"/>
       <c r="D30" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" s="36"/>
+      <c r="B31" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="35"/>
       <c r="D31" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="36"/>
+      <c r="B32" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="35"/>
       <c r="D32" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" s="36"/>
+      <c r="B33" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="35"/>
       <c r="D33" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="36"/>
+      <c r="B34" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="35"/>
       <c r="D34" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C35" s="36"/>
+      <c r="B35" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="35"/>
       <c r="D35" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="36"/>
+      <c r="B36" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="35"/>
       <c r="D36" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="36"/>
+      <c r="B37" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="35"/>
       <c r="D37" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
       <c r="D39" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
       <c r="D40" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="36"/>
+        <v>82</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="35"/>
       <c r="D41" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
+        <v>80</v>
+      </c>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
       <c r="D42" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="36"/>
+      <c r="B43" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="35"/>
       <c r="D43" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
       <c r="D44" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
+        <v>39</v>
+      </c>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
       <c r="D45" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
+      <c r="A46" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
       <c r="D46" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="C47" s="36"/>
+      <c r="A47" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
       <c r="D47" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
+      <c r="A48" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
       <c r="D48" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="A49" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" s="42"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="41"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
+      <c r="A50" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="35"/>
       <c r="D50" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="42" t="s">
+      <c r="A51" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" s="35"/>
+      <c r="D51" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="42"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="31" t="s">
+      <c r="B52" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="35"/>
+      <c r="D52" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="36" t="s">
+      <c r="B53" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="35"/>
+      <c r="D53" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" s="44"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="43"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="C53" s="36"/>
-      <c r="D53" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="36" t="s">
+      <c r="B55" s="30"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B54" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" s="36"/>
-      <c r="D54" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="B55" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" s="36"/>
-      <c r="D55" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="44"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="B57" s="31"/>
-      <c r="C57" s="36"/>
+        <v>102</v>
+      </c>
+      <c r="B57" s="35"/>
+      <c r="C57" s="35"/>
       <c r="D57" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
+      <c r="A58" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" s="35"/>
+      <c r="C58" s="35"/>
       <c r="D58" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
+        <v>98</v>
+      </c>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
       <c r="D59" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
+        <v>99</v>
+      </c>
+      <c r="B60" s="35"/>
+      <c r="C60" s="35"/>
       <c r="D60" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="D61"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D63"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D64"/>
+      <c r="D62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1786,467 +1752,467 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="69.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="45" style="41" customWidth="1"/>
+    <col min="2" max="3" width="45" style="40" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="11.5546875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="38" t="s">
+      <c r="A1" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>77</v>
+      <c r="C1" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="30"/>
+      <c r="A2" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="29"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
+        <v>42</v>
+      </c>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
       <c r="D3" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
+        <v>43</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
+        <v>44</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
+        <v>100</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="30"/>
+      <c r="A7" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
+        <v>46</v>
+      </c>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
+        <v>47</v>
+      </c>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
+        <v>48</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
+        <v>49</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
+        <v>44</v>
+      </c>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
       <c r="D12" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="30"/>
+        <v>50</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="29"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
+        <v>51</v>
+      </c>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
+        <v>52</v>
+      </c>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
+        <v>53</v>
+      </c>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
+        <v>54</v>
+      </c>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="30"/>
+        <v>55</v>
+      </c>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="29"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
+        <v>100</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
+        <v>51</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
+        <v>56</v>
+      </c>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
+        <v>57</v>
+      </c>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
+        <v>58</v>
+      </c>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
+        <v>59</v>
+      </c>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
       <c r="D24" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="30"/>
+        <v>60</v>
+      </c>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="29"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
+        <v>100</v>
+      </c>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
       <c r="D26" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
+        <v>61</v>
+      </c>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
       <c r="D27" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
+        <v>62</v>
+      </c>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
       <c r="D28" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
       <c r="D29" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
+        <v>56</v>
+      </c>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
       <c r="D30" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="30"/>
+        <v>64</v>
+      </c>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="29"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
+        <v>105</v>
+      </c>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
       <c r="D32" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
+        <v>100</v>
+      </c>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
       <c r="D33" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
+        <v>51</v>
+      </c>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
       <c r="D34" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
+        <v>56</v>
+      </c>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
       <c r="D35" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
+        <v>65</v>
+      </c>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
       <c r="D36" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="46"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="48" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="30"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="29"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
+        <v>100</v>
+      </c>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
       <c r="D40" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
+        <v>51</v>
+      </c>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
       <c r="D41" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
+        <v>56</v>
+      </c>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
       <c r="D42" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
+        <v>69</v>
+      </c>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
       <c r="D43" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="30"/>
+      <c r="A44" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="29"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
+        <v>107</v>
+      </c>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
       <c r="D45" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
+      <c r="A46" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B47" s="39"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
+        <v>70</v>
+      </c>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>